<commit_message>
add função para formatar o cpf
</commit_message>
<xml_diff>
--- a/api/tmp/file.xlsx
+++ b/api/tmp/file.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23416"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_92485C45C1F39E42E268565A893E8C18510380CC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9040F3FB-5A56-4F97-B731-C64DD26FAAB6}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandre\Documents\Teste-expense-mobi\api\tmp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,31 +30,82 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="6">
-  <si>
-    <t>nome</t>
-  </si>
-  <si>
-    <t>sobrenome</t>
-  </si>
-  <si>
-    <t>cpf</t>
-  </si>
-  <si>
-    <t>Alexandre</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Ribeiro</t>
   </si>
   <si>
     <t>115.853.176-16</t>
+  </si>
+  <si>
+    <t>Alexandre1</t>
+  </si>
+  <si>
+    <t>Alexandre2</t>
+  </si>
+  <si>
+    <t>Alexandre3</t>
+  </si>
+  <si>
+    <t>Alexandre4</t>
+  </si>
+  <si>
+    <t>Alexandre5</t>
+  </si>
+  <si>
+    <t>Alexandre6</t>
+  </si>
+  <si>
+    <t>Alexandre7</t>
+  </si>
+  <si>
+    <t>Alexandre8</t>
+  </si>
+  <si>
+    <t>Alexandre9</t>
+  </si>
+  <si>
+    <t>Alexandre10</t>
+  </si>
+  <si>
+    <t>Alexandre11</t>
+  </si>
+  <si>
+    <t>115.853.176-17</t>
+  </si>
+  <si>
+    <t>115.853.176-18</t>
+  </si>
+  <si>
+    <t>115.853.176-19</t>
+  </si>
+  <si>
+    <t>115.853.176-20</t>
+  </si>
+  <si>
+    <t>115.853.176-21</t>
+  </si>
+  <si>
+    <t>115.853.176-22</t>
+  </si>
+  <si>
+    <t>115.853.176-23</t>
+  </si>
+  <si>
+    <t>115.853.176-24</t>
+  </si>
+  <si>
+    <t>115.853.176-25</t>
+  </si>
+  <si>
+    <t>115.853.176-26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,149 +458,145 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:D12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>